<commit_message>
Updated source data with folders
</commit_message>
<xml_diff>
--- a/AI model Power Consumption Database - with graphs.xlsx
+++ b/AI model Power Consumption Database - with graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snarayan\Downloads\model_training_resource_consumption_benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEB3DF5-6A20-4114-9104-E6FB601F89D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8702059-472A-4A60-A77A-0C845CBAC00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{63DAF364-F857-4F0A-938E-B54295742752}"/>
   </bookViews>
@@ -567,6 +567,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-76E9-4DAD-A9AA-072D7B244B7D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -896,6 +901,9 @@
                     </c:manualLayout>
                   </c15:layout>
                   <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-76E9-4DAD-A9AA-072D7B244B7D}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1327,6 +1335,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-32B9-44C8-B6CA-9005920547C6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -1755,6 +1768,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-0AF3-4627-9DDD-979A00B95881}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -1919,6 +1937,9 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-0AF3-4627-9DDD-979A00B95881}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2360,6 +2381,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-F488-433C-B016-55FE49073580}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -2643,6 +2669,9 @@
                   </c15:layout>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-F488-433C-B016-55FE49073580}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -3074,6 +3103,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-7BD8-4CED-BF9E-790AC6154653}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -3407,6 +3441,9 @@
                   </c15:layout>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-7BD8-4CED-BF9E-790AC6154653}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -3845,6 +3882,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-30EC-4D16-A0A6-8BA36364B30D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -7934,7 +7976,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7766BABF-5672-41FA-8635-C262FC3FAC3D}">
   <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I57" sqref="I57"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>